<commit_message>
- Thêm cột thời gian điểm danh ra cho bảng sự kiện. Cập nhật cơ sở dữ liệu. - Cập nhật lại các file import đăng ký sự kiện. - Kiểm tra thời gian điểm danh ra cập nhật tự động cho chức năng điểm danh.
</commit_message>
<xml_diff>
--- a/Sources/DD_RFID/public/download/Mẫu đăng ký sự kiện.xlsx
+++ b/Sources/DD_RFID/public/download/Mẫu đăng ký sự kiện.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>mssv</t>
   </si>
@@ -100,43 +100,7 @@
     <t>K41</t>
   </si>
   <si>
-    <t>Trần Văn Bình</t>
-  </si>
-  <si>
     <t>Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>vanb@gmail.com</t>
-  </si>
-  <si>
-    <t>Phan Công Huy</t>
-  </si>
-  <si>
-    <t>pchuy@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Thị Hậu</t>
-  </si>
-  <si>
-    <t>hau@hotmail.com</t>
-  </si>
-  <si>
-    <t>Nguyễn Chín</t>
-  </si>
-  <si>
-    <t>chin@email.com</t>
-  </si>
-  <si>
-    <t>00123457</t>
-  </si>
-  <si>
-    <t>00123458</t>
-  </si>
-  <si>
-    <t>00123459</t>
-  </si>
-  <si>
-    <t>00123460</t>
   </si>
   <si>
     <t>HƯỚNG DẪN SỬ DỤNG FILE IMPORT DỮ LIỆU MẪU.</t>
@@ -294,6 +258,15 @@
   </si>
   <si>
     <t>- Tốc độ import sẽ chậm dần theo thứ tự định dạng như sau: csv (nhanh nhất) &gt; xls &gt; xlsx</t>
+  </si>
+  <si>
+    <t>Nguyễn Ân Hiên</t>
+  </si>
+  <si>
+    <t>vana@gmail.com</t>
+  </si>
+  <si>
+    <t>00123456</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1154,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1215,7 +1188,7 @@
     </row>
     <row r="5" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1236,7 +1209,7 @@
     <row r="6" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1256,7 +1229,7 @@
     <row r="7" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="11" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -1276,7 +1249,7 @@
     <row r="8" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -1296,7 +1269,7 @@
     <row r="9" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="11" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -1316,7 +1289,7 @@
     <row r="10" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="11" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -1353,7 +1326,7 @@
     </row>
     <row r="12" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1374,7 +1347,7 @@
     <row r="13" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" s="13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1394,7 +1367,7 @@
     <row r="14" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="13" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1414,7 +1387,7 @@
     <row r="15" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1812,7 +1785,7 @@
     <row r="37" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -1832,7 +1805,7 @@
     <row r="38" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="13" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -2117,7 +2090,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2149,82 +2122,32 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576">
       <formula1>BOMON</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576">
       <formula1>khoa</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2624,19 +2547,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2644,7 +2567,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
@@ -2654,22 +2577,22 @@
         <v>K43</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D11" ca="1" si="0">"K" &amp; TEXT( YEAR( TODAY()) - (ROW()+1972), "0")</f>
         <v>K42</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2692,7 +2615,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2707,7 +2630,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2719,22 +2642,22 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>K38</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2743,7 +2666,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2752,7 +2675,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" ca="1" si="0"/>

</xml_diff>